<commit_message>
added About page with turtled image
</commit_message>
<xml_diff>
--- a/P07/Scrum_Sprint_2.xlsx
+++ b/P07/Scrum_Sprint_2.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcnar\Desktop\cse1325\P06\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcnar\Desktop\cse1325\P07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95C0E4F-25F2-4754-84DD-75954C50BCCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67BB329-2B45-4821-8E45-9B8772259F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Sprint 02 Backlog" sheetId="3" r:id="rId2"/>
-    <sheet name="Sprint 01 Backlog" sheetId="2" r:id="rId3"/>
-    <sheet name="Sprint 03 Backlog" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint 03 Backlog" sheetId="4" r:id="rId2"/>
+    <sheet name="Sprint 02 Backlog" sheetId="3" r:id="rId3"/>
+    <sheet name="Sprint 01 Backlog" sheetId="2" r:id="rId4"/>
     <sheet name="Sprint 04 Backlog" sheetId="5" r:id="rId5"/>
     <sheet name="Sprint 05 Backlog" sheetId="6" r:id="rId6"/>
     <sheet name="Sprint 06 Backlog" sheetId="7" r:id="rId7"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="206">
   <si>
     <t>Product Name:</t>
   </si>
@@ -651,6 +651,15 @@
   </si>
   <si>
     <t>Completed Day 5</t>
+  </si>
+  <si>
+    <t>Create About Diolog for Photos</t>
+  </si>
+  <si>
+    <t>Finished in Sprint 3</t>
+  </si>
+  <si>
+    <t>Create turtle image using template in 1325-prof</t>
   </si>
 </sst>
 </file>
@@ -1189,13 +1198,13 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1384,6 +1393,320 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:style val="2"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1300" b="0" strike="noStrike" spc="-1">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Sprint Burn Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:separator>; </c:separator>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 03 Backlog'!$B$7:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D9A3-4FA9-8103-4B161ABEFDBB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:smooth val="0"/>
+        <c:axId val="62406455"/>
+        <c:axId val="96539211"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="62406455"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Days</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="B3B3B3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="96539211"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="96539211"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="0">
+              <a:solidFill>
+                <a:srgbClr val="B3B3B3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Tasks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="B3B3B3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="62406455"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:solidFill>
+            <a:srgbClr val="B3B3B3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="0">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1697,7 +2020,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1979,320 +2302,6 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="30947722"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="B3B3B3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
-    </a:solidFill>
-    <a:ln w="0">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:style val="2"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1300" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Sprint Burn Chart</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
-            <c:separator>; </c:separator>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Sprint 03 Backlog'!$B$7:$B$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D9A3-4FA9-8103-4B161ABEFDBB}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:smooth val="0"/>
-        <c:axId val="62406455"/>
-        <c:axId val="96539211"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="62406455"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Days</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="B3B3B3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="96539211"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="96539211"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="B3B3B3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Tasks</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="B3B3B3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="62406455"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3325,10 +3334,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3359,8 +3368,8 @@
       <xdr:rowOff>67680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1773000</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>518400</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>134280</xdr:rowOff>
     </xdr:to>
@@ -3369,7 +3378,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3400,17 +3409,17 @@
       <xdr:rowOff>67680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1773000</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>134280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3856,8 +3865,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView topLeftCell="A27" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4115,11 +4124,11 @@
       </c>
       <c r="B15" s="5">
         <f>B14-C15</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C15" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 3")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="5"/>
@@ -4139,7 +4148,7 @@
       </c>
       <c r="B16" s="5">
         <f>B15-C16</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C16" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 4")</f>
@@ -4159,7 +4168,7 @@
       </c>
       <c r="B17" s="5">
         <f>B16-C17</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C17" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 4")</f>
@@ -4643,8 +4652,12 @@
       <c r="E35" s="42">
         <v>2</v>
       </c>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
+      <c r="F35" s="17">
+        <v>3</v>
+      </c>
+      <c r="G35" s="17" t="s">
+        <v>204</v>
+      </c>
       <c r="H35" s="18" t="s">
         <v>70</v>
       </c>
@@ -4672,8 +4685,12 @@
       <c r="E36" s="16">
         <v>5</v>
       </c>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
+      <c r="F36" s="17">
+        <v>3</v>
+      </c>
+      <c r="G36" s="17" t="s">
+        <v>204</v>
+      </c>
       <c r="H36" s="18" t="s">
         <v>70</v>
       </c>
@@ -4701,7 +4718,9 @@
       <c r="E37" s="16">
         <v>13</v>
       </c>
-      <c r="F37" s="17"/>
+      <c r="F37" s="17">
+        <v>3</v>
+      </c>
       <c r="G37" s="17"/>
       <c r="H37" s="18" t="s">
         <v>79</v>
@@ -4730,7 +4749,9 @@
       <c r="E38" s="16">
         <v>1</v>
       </c>
-      <c r="F38" s="17"/>
+      <c r="F38" s="17">
+        <v>3</v>
+      </c>
       <c r="G38" s="17"/>
       <c r="H38" s="18" t="s">
         <v>79</v>
@@ -4759,7 +4780,9 @@
       <c r="E39" s="16">
         <v>5</v>
       </c>
-      <c r="F39" s="17"/>
+      <c r="F39" s="17">
+        <v>3</v>
+      </c>
       <c r="G39" s="17"/>
       <c r="H39" s="18" t="s">
         <v>79</v>
@@ -4788,7 +4811,9 @@
       <c r="E40" s="16">
         <v>8</v>
       </c>
-      <c r="F40" s="17"/>
+      <c r="F40" s="17">
+        <v>3</v>
+      </c>
       <c r="G40" s="17"/>
       <c r="H40" s="18" t="s">
         <v>79</v>
@@ -5807,6 +5832,1190 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AMJ100"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="51.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="51.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1024" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="25">
+        <f>'Sprint 02 Backlog'!B1+1</f>
+        <v>3</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1"/>
+      <c r="F1" s="25"/>
+      <c r="AMI1"/>
+      <c r="AMJ1"/>
+    </row>
+    <row r="2" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="29">
+        <f>'Sprint 02 Backlog'!B2+7</f>
+        <v>44992</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="30" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="AMI2"/>
+      <c r="AMJ2"/>
+    </row>
+    <row r="3" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="29">
+        <f>B2+14</f>
+        <v>45006</v>
+      </c>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="AMI3"/>
+      <c r="AMJ3"/>
+    </row>
+    <row r="4" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="AMI4"/>
+      <c r="AMJ4"/>
+    </row>
+    <row r="5" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="25"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="AMI5"/>
+      <c r="AMJ5"/>
+    </row>
+    <row r="6" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="25"/>
+      <c r="B6" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="AMI6"/>
+      <c r="AMJ6"/>
+    </row>
+    <row r="7" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="25">
+        <f>COUNTA(D17:D995)</f>
+        <v>2</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="AMI7"/>
+      <c r="AMJ7"/>
+    </row>
+    <row r="8" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="25">
+        <f t="shared" ref="B8:B14" si="0">B7-C8</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="25">
+        <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
+        <v>2</v>
+      </c>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="AMI8"/>
+      <c r="AMJ8"/>
+    </row>
+    <row r="9" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B9" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C9" s="25">
+        <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="AMI9"/>
+      <c r="AMJ9"/>
+    </row>
+    <row r="10" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C10" s="25">
+        <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="AMI10"/>
+      <c r="AMJ10"/>
+    </row>
+    <row r="11" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C11" s="25">
+        <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="AMI11"/>
+      <c r="AMJ11"/>
+    </row>
+    <row r="12" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="B12" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C12" s="25">
+        <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="AMI12"/>
+      <c r="AMJ12"/>
+    </row>
+    <row r="13" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="B13" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C13" s="25">
+        <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="AMI13"/>
+      <c r="AMJ13"/>
+    </row>
+    <row r="14" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C14" s="25">
+        <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="AMI14"/>
+      <c r="AMJ14"/>
+    </row>
+    <row r="15" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="25"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="AMI15"/>
+      <c r="AMJ15"/>
+    </row>
+    <row r="16" spans="1:1024" x14ac:dyDescent="0.2">
+      <c r="A16" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>1</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D17" s="44" t="s">
+        <v>203</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="F17" s="38"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>2</v>
+      </c>
+      <c r="B18" s="35"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="38"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>3</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D19" s="39" t="s">
+        <v>205</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="F19" s="38"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>4</v>
+      </c>
+      <c r="B20" s="35"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="38"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>5</v>
+      </c>
+      <c r="B21" s="35"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="38"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>6</v>
+      </c>
+      <c r="B22" s="35"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="38"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>7</v>
+      </c>
+      <c r="B23" s="35"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="38"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
+        <v>8</v>
+      </c>
+      <c r="B24" s="35"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="38"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>9</v>
+      </c>
+      <c r="B25" s="35"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="38"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>10</v>
+      </c>
+      <c r="B26" s="35"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="38"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
+        <v>11</v>
+      </c>
+      <c r="B27" s="35"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="38"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
+        <v>12</v>
+      </c>
+      <c r="B28" s="35"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="38"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <v>13</v>
+      </c>
+      <c r="B29" s="35"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="38"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>14</v>
+      </c>
+      <c r="B30" s="35"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="38"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
+        <v>15</v>
+      </c>
+      <c r="B31" s="35"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="38"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
+        <v>16</v>
+      </c>
+      <c r="B32" s="35"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="38"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="4">
+        <v>17</v>
+      </c>
+      <c r="B33" s="35"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="38"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="4">
+        <v>18</v>
+      </c>
+      <c r="B34" s="35"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="38"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="4">
+        <v>19</v>
+      </c>
+      <c r="B35" s="35"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="38"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="4">
+        <v>20</v>
+      </c>
+      <c r="B36" s="35"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="38"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="4">
+        <v>21</v>
+      </c>
+      <c r="B37" s="35"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="38"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="4">
+        <v>22</v>
+      </c>
+      <c r="B38" s="35"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="38"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="4">
+        <v>23</v>
+      </c>
+      <c r="B39" s="35"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="38"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="4">
+        <v>24</v>
+      </c>
+      <c r="B40" s="35"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="38"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="4">
+        <v>25</v>
+      </c>
+      <c r="B41" s="35"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="38"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="4">
+        <v>26</v>
+      </c>
+      <c r="B42" s="35"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="37"/>
+      <c r="F42" s="38"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="4">
+        <v>27</v>
+      </c>
+      <c r="B43" s="35"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="38"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="4">
+        <v>28</v>
+      </c>
+      <c r="B44" s="35"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="38"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="4">
+        <v>29</v>
+      </c>
+      <c r="B45" s="35"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="38"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="4">
+        <v>30</v>
+      </c>
+      <c r="B46" s="35"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="38"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="4">
+        <v>31</v>
+      </c>
+      <c r="B47" s="35"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="38"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="4">
+        <v>32</v>
+      </c>
+      <c r="B48" s="35"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="38"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="4">
+        <v>33</v>
+      </c>
+      <c r="B49" s="35"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="38"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="4">
+        <v>34</v>
+      </c>
+      <c r="B50" s="35"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="37"/>
+      <c r="F50" s="38"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="4">
+        <v>35</v>
+      </c>
+      <c r="B51" s="35"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="39"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="38"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="4">
+        <v>36</v>
+      </c>
+      <c r="B52" s="35"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="39"/>
+      <c r="E52" s="37"/>
+      <c r="F52" s="38"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="4">
+        <v>37</v>
+      </c>
+      <c r="B53" s="35"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="38"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="4">
+        <v>38</v>
+      </c>
+      <c r="B54" s="35"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="39"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="38"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="4">
+        <v>39</v>
+      </c>
+      <c r="B55" s="35"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="38"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="4">
+        <v>40</v>
+      </c>
+      <c r="B56" s="35"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="38"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="4">
+        <v>41</v>
+      </c>
+      <c r="B57" s="35"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="39"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="38"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="4">
+        <v>42</v>
+      </c>
+      <c r="B58" s="35"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="38"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="4">
+        <v>43</v>
+      </c>
+      <c r="B59" s="35"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="39"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="38"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="4">
+        <v>44</v>
+      </c>
+      <c r="B60" s="35"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="39"/>
+      <c r="E60" s="37"/>
+      <c r="F60" s="38"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="4">
+        <v>45</v>
+      </c>
+      <c r="B61" s="35"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="39"/>
+      <c r="E61" s="37"/>
+      <c r="F61" s="38"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="4">
+        <v>46</v>
+      </c>
+      <c r="B62" s="35"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="39"/>
+      <c r="E62" s="37"/>
+      <c r="F62" s="38"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="4">
+        <v>47</v>
+      </c>
+      <c r="B63" s="35"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="39"/>
+      <c r="E63" s="37"/>
+      <c r="F63" s="38"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="4">
+        <v>48</v>
+      </c>
+      <c r="B64" s="35"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="37"/>
+      <c r="F64" s="38"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="4">
+        <v>49</v>
+      </c>
+      <c r="B65" s="35"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="39"/>
+      <c r="E65" s="37"/>
+      <c r="F65" s="38"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="4">
+        <v>50</v>
+      </c>
+      <c r="B66" s="35"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="39"/>
+      <c r="E66" s="37"/>
+      <c r="F66" s="38"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="4">
+        <v>51</v>
+      </c>
+      <c r="B67" s="35"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="39"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="38"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="4">
+        <v>52</v>
+      </c>
+      <c r="B68" s="35"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="37"/>
+      <c r="F68" s="38"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="4">
+        <v>53</v>
+      </c>
+      <c r="B69" s="35"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="39"/>
+      <c r="E69" s="37"/>
+      <c r="F69" s="38"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="4">
+        <v>54</v>
+      </c>
+      <c r="B70" s="35"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="39"/>
+      <c r="E70" s="37"/>
+      <c r="F70" s="38"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="4">
+        <v>55</v>
+      </c>
+      <c r="B71" s="35"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="39"/>
+      <c r="E71" s="37"/>
+      <c r="F71" s="38"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="4">
+        <v>56</v>
+      </c>
+      <c r="B72" s="35"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="39"/>
+      <c r="E72" s="37"/>
+      <c r="F72" s="38"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="4">
+        <v>57</v>
+      </c>
+      <c r="B73" s="35"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="39"/>
+      <c r="E73" s="37"/>
+      <c r="F73" s="38"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="4">
+        <v>58</v>
+      </c>
+      <c r="B74" s="35"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="39"/>
+      <c r="E74" s="37"/>
+      <c r="F74" s="38"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="4">
+        <v>59</v>
+      </c>
+      <c r="B75" s="35"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="39"/>
+      <c r="E75" s="37"/>
+      <c r="F75" s="38"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="4">
+        <v>60</v>
+      </c>
+      <c r="B76" s="35"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="39"/>
+      <c r="E76" s="37"/>
+      <c r="F76" s="38"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="4">
+        <v>61</v>
+      </c>
+      <c r="B77" s="35"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="39"/>
+      <c r="E77" s="37"/>
+      <c r="F77" s="38"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="4">
+        <v>62</v>
+      </c>
+      <c r="B78" s="35"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="39"/>
+      <c r="E78" s="37"/>
+      <c r="F78" s="38"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="4">
+        <v>63</v>
+      </c>
+      <c r="B79" s="35"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="39"/>
+      <c r="E79" s="37"/>
+      <c r="F79" s="38"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="4">
+        <v>64</v>
+      </c>
+      <c r="B80" s="35"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="39"/>
+      <c r="E80" s="37"/>
+      <c r="F80" s="38"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="4">
+        <v>65</v>
+      </c>
+      <c r="B81" s="35"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="39"/>
+      <c r="E81" s="37"/>
+      <c r="F81" s="38"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="4">
+        <v>66</v>
+      </c>
+      <c r="B82" s="35"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="39"/>
+      <c r="E82" s="37"/>
+      <c r="F82" s="38"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="4">
+        <v>67</v>
+      </c>
+      <c r="B83" s="35"/>
+      <c r="C83" s="4"/>
+      <c r="D83" s="39"/>
+      <c r="E83" s="37"/>
+      <c r="F83" s="38"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="4">
+        <v>68</v>
+      </c>
+      <c r="B84" s="35"/>
+      <c r="C84" s="4"/>
+      <c r="D84" s="39"/>
+      <c r="E84" s="37"/>
+      <c r="F84" s="38"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="4">
+        <v>69</v>
+      </c>
+      <c r="B85" s="35"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="39"/>
+      <c r="E85" s="37"/>
+      <c r="F85" s="38"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="4">
+        <v>70</v>
+      </c>
+      <c r="B86" s="35"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="39"/>
+      <c r="E86" s="37"/>
+      <c r="F86" s="38"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="4">
+        <v>71</v>
+      </c>
+      <c r="B87" s="35"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="39"/>
+      <c r="E87" s="37"/>
+      <c r="F87" s="38"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="4">
+        <v>72</v>
+      </c>
+      <c r="B88" s="35"/>
+      <c r="C88" s="4"/>
+      <c r="D88" s="39"/>
+      <c r="E88" s="37"/>
+      <c r="F88" s="38"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="4">
+        <v>73</v>
+      </c>
+      <c r="B89" s="35"/>
+      <c r="C89" s="4"/>
+      <c r="D89" s="39"/>
+      <c r="E89" s="37"/>
+      <c r="F89" s="38"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="4">
+        <v>74</v>
+      </c>
+      <c r="B90" s="35"/>
+      <c r="C90" s="4"/>
+      <c r="D90" s="39"/>
+      <c r="E90" s="37"/>
+      <c r="F90" s="38"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="4">
+        <v>75</v>
+      </c>
+      <c r="B91" s="35"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="39"/>
+      <c r="E91" s="37"/>
+      <c r="F91" s="38"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="4">
+        <v>76</v>
+      </c>
+      <c r="B92" s="35"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="39"/>
+      <c r="E92" s="37"/>
+      <c r="F92" s="38"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="4">
+        <v>77</v>
+      </c>
+      <c r="B93" s="35"/>
+      <c r="C93" s="4"/>
+      <c r="D93" s="39"/>
+      <c r="E93" s="37"/>
+      <c r="F93" s="38"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="4">
+        <v>78</v>
+      </c>
+      <c r="B94" s="35"/>
+      <c r="C94" s="4"/>
+      <c r="D94" s="39"/>
+      <c r="E94" s="37"/>
+      <c r="F94" s="38"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="4">
+        <v>79</v>
+      </c>
+      <c r="B95" s="35"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="39"/>
+      <c r="E95" s="37"/>
+      <c r="F95" s="38"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="4">
+        <v>80</v>
+      </c>
+      <c r="B96" s="35"/>
+      <c r="C96" s="4"/>
+      <c r="D96" s="39"/>
+      <c r="E96" s="37"/>
+      <c r="F96" s="38"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="4">
+        <v>81</v>
+      </c>
+      <c r="B97" s="35"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="39"/>
+      <c r="E97" s="37"/>
+      <c r="F97" s="38"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="4">
+        <v>82</v>
+      </c>
+      <c r="B98" s="35"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="39"/>
+      <c r="E98" s="37"/>
+      <c r="F98" s="38"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" s="4">
+        <v>83</v>
+      </c>
+      <c r="B99" s="35"/>
+      <c r="C99" s="4"/>
+      <c r="D99" s="39"/>
+      <c r="E99" s="37"/>
+      <c r="F99" s="38"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" s="4">
+        <v>84</v>
+      </c>
+      <c r="B100" s="35"/>
+      <c r="C100" s="4"/>
+      <c r="D100" s="39"/>
+      <c r="E100" s="37"/>
+      <c r="F100" s="38"/>
+    </row>
+  </sheetData>
+  <dataValidations xWindow="221" yWindow="736" count="4">
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task ID" prompt="This is just an arbitrary unique (per sprint) integer assigned to a task, used by the team to refer to that task. " sqref="A17:A100" xr:uid="{00000000-0002-0000-0300-000000000000}">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature._x000a__x000a_Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" sqref="D18:D100" xr:uid="{00000000-0002-0000-0300-000003000000}">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" promptTitle="Implementation Status" prompt="Leave blank until task is begun._x000a_Select &quot;In Work&quot; when started (for long tasks only)._x000a_Select Completed ONLY when this task is done._x000a_    Select &quot;Completed Day 1&quot; if finished on the first day, and_x000a_    similarly for &quot;Completed on Day 2&quot; et. al." sqref="E17:E100" xr:uid="{00000000-0002-0000-0300-000004000000}">
+      <formula1>"In Work,Completed Day 1,Completed Day 2,Completed Day 3,Completed Day 4,Completed Day 5,Completed Day 6,Completed Day 7"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F17:F100" xr:uid="{00000000-0002-0000-0300-000005000000}">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="221" yWindow="736" count="2">
+        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="Exactly ONE team member may be responsible for any task, and they will receive grade credit for their work._x000a__x000a_If you have more than one person on your team, each member MUST select their initials for each task the agree to perform. Use this to ensure that " xr:uid="{00000000-0002-0000-0300-000002000000}">
+          <x14:formula1>
+            <xm:f>'Product Backlog'!$H$5:$H$9</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>C17:C100</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="The list contains the Feature IDs from the same column on the Product Backlog tab._x000a__x000a_For each (ahem) Feature ID, create one or more rows in this table representing the tasks you need to complete to implement that feature._x000a__x000a_For example, for a &quot;Provide Help " xr:uid="{00000000-0002-0000-0300-000001000000}">
+          <x14:formula1>
+            <xm:f>'Product Backlog'!$A$24:$A$100</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>B17:B100</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
@@ -7134,7 +8343,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
@@ -8485,1176 +9694,6 @@
             <xm:f>0</xm:f>
           </x14:formula2>
           <xm:sqref>B45:B100</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMJ100"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="51.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="51.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1024" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="25">
-        <f>'Sprint 02 Backlog'!B1+1</f>
-        <v>3</v>
-      </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1"/>
-      <c r="F1" s="25"/>
-      <c r="AMI1"/>
-      <c r="AMJ1"/>
-    </row>
-    <row r="2" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="B2" s="29">
-        <f>'Sprint 02 Backlog'!B2+7</f>
-        <v>44992</v>
-      </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="AMI2"/>
-      <c r="AMJ2"/>
-    </row>
-    <row r="3" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="B3" s="29">
-        <f>B2+14</f>
-        <v>45006</v>
-      </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="AMI3"/>
-      <c r="AMJ3"/>
-    </row>
-    <row r="4" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="AMI4"/>
-      <c r="AMJ4"/>
-    </row>
-    <row r="5" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="25"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="AMI5"/>
-      <c r="AMJ5"/>
-    </row>
-    <row r="6" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="25"/>
-      <c r="B6" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>137</v>
-      </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="AMI6"/>
-      <c r="AMJ6"/>
-    </row>
-    <row r="7" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="B7" s="25">
-        <f>COUNTA(D17:D995)</f>
-        <v>1</v>
-      </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="AMI7"/>
-      <c r="AMJ7"/>
-    </row>
-    <row r="8" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="B8" s="25">
-        <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>1</v>
-      </c>
-      <c r="C8" s="25">
-        <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="AMI8"/>
-      <c r="AMJ8"/>
-    </row>
-    <row r="9" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="25" t="s">
-        <v>140</v>
-      </c>
-      <c r="B9" s="25">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C9" s="25">
-        <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="AMI9"/>
-      <c r="AMJ9"/>
-    </row>
-    <row r="10" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="B10" s="25">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C10" s="25">
-        <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="AMI10"/>
-      <c r="AMJ10"/>
-    </row>
-    <row r="11" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="B11" s="25">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C11" s="25">
-        <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="AMI11"/>
-      <c r="AMJ11"/>
-    </row>
-    <row r="12" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="B12" s="25">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C12" s="25">
-        <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="AMI12"/>
-      <c r="AMJ12"/>
-    </row>
-    <row r="13" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="B13" s="25">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C13" s="25">
-        <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="AMI13"/>
-      <c r="AMJ13"/>
-    </row>
-    <row r="14" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="B14" s="25">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C14" s="25">
-        <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="AMI14"/>
-      <c r="AMJ14"/>
-    </row>
-    <row r="15" spans="1:1024" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="AMI15"/>
-      <c r="AMJ15"/>
-    </row>
-    <row r="16" spans="1:1024" x14ac:dyDescent="0.2">
-      <c r="A16" s="33" t="s">
-        <v>146</v>
-      </c>
-      <c r="B16" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="33" t="s">
-        <v>147</v>
-      </c>
-      <c r="D16" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="E16" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
-        <v>1</v>
-      </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="36" t="s">
-        <v>149</v>
-      </c>
-      <c r="E17" s="37"/>
-      <c r="F17" s="38"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
-        <v>2</v>
-      </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="38"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
-        <v>3</v>
-      </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="38"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
-        <v>4</v>
-      </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="38"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
-        <v>5</v>
-      </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="38"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
-        <v>6</v>
-      </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="38"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
-        <v>7</v>
-      </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="38"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
-        <v>8</v>
-      </c>
-      <c r="B24" s="35"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="38"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="4">
-        <v>9</v>
-      </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="38"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="4">
-        <v>10</v>
-      </c>
-      <c r="B26" s="35"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="38"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="4">
-        <v>11</v>
-      </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="38"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
-        <v>12</v>
-      </c>
-      <c r="B28" s="35"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="38"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="4">
-        <v>13</v>
-      </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="38"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="4">
-        <v>14</v>
-      </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="38"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="4">
-        <v>15</v>
-      </c>
-      <c r="B31" s="35"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="38"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="4">
-        <v>16</v>
-      </c>
-      <c r="B32" s="35"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="38"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="4">
-        <v>17</v>
-      </c>
-      <c r="B33" s="35"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="38"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="4">
-        <v>18</v>
-      </c>
-      <c r="B34" s="35"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="38"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="4">
-        <v>19</v>
-      </c>
-      <c r="B35" s="35"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="38"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="4">
-        <v>20</v>
-      </c>
-      <c r="B36" s="35"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="38"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="4">
-        <v>21</v>
-      </c>
-      <c r="B37" s="35"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="39"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="38"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="4">
-        <v>22</v>
-      </c>
-      <c r="B38" s="35"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="38"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="4">
-        <v>23</v>
-      </c>
-      <c r="B39" s="35"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="39"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="38"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="4">
-        <v>24</v>
-      </c>
-      <c r="B40" s="35"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="38"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="4">
-        <v>25</v>
-      </c>
-      <c r="B41" s="35"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="39"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="38"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="4">
-        <v>26</v>
-      </c>
-      <c r="B42" s="35"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="39"/>
-      <c r="E42" s="37"/>
-      <c r="F42" s="38"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="4">
-        <v>27</v>
-      </c>
-      <c r="B43" s="35"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="38"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="4">
-        <v>28</v>
-      </c>
-      <c r="B44" s="35"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="39"/>
-      <c r="E44" s="37"/>
-      <c r="F44" s="38"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="4">
-        <v>29</v>
-      </c>
-      <c r="B45" s="35"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="38"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="4">
-        <v>30</v>
-      </c>
-      <c r="B46" s="35"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="37"/>
-      <c r="F46" s="38"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="4">
-        <v>31</v>
-      </c>
-      <c r="B47" s="35"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="39"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="38"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="4">
-        <v>32</v>
-      </c>
-      <c r="B48" s="35"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="39"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="38"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="4">
-        <v>33</v>
-      </c>
-      <c r="B49" s="35"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="39"/>
-      <c r="E49" s="37"/>
-      <c r="F49" s="38"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="4">
-        <v>34</v>
-      </c>
-      <c r="B50" s="35"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="39"/>
-      <c r="E50" s="37"/>
-      <c r="F50" s="38"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="4">
-        <v>35</v>
-      </c>
-      <c r="B51" s="35"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="39"/>
-      <c r="E51" s="37"/>
-      <c r="F51" s="38"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="4">
-        <v>36</v>
-      </c>
-      <c r="B52" s="35"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="39"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="38"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="4">
-        <v>37</v>
-      </c>
-      <c r="B53" s="35"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="39"/>
-      <c r="E53" s="37"/>
-      <c r="F53" s="38"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="4">
-        <v>38</v>
-      </c>
-      <c r="B54" s="35"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="39"/>
-      <c r="E54" s="37"/>
-      <c r="F54" s="38"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="4">
-        <v>39</v>
-      </c>
-      <c r="B55" s="35"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="39"/>
-      <c r="E55" s="37"/>
-      <c r="F55" s="38"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="4">
-        <v>40</v>
-      </c>
-      <c r="B56" s="35"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="39"/>
-      <c r="E56" s="37"/>
-      <c r="F56" s="38"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="4">
-        <v>41</v>
-      </c>
-      <c r="B57" s="35"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="39"/>
-      <c r="E57" s="37"/>
-      <c r="F57" s="38"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="4">
-        <v>42</v>
-      </c>
-      <c r="B58" s="35"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="39"/>
-      <c r="E58" s="37"/>
-      <c r="F58" s="38"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="4">
-        <v>43</v>
-      </c>
-      <c r="B59" s="35"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="39"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="38"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="4">
-        <v>44</v>
-      </c>
-      <c r="B60" s="35"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="39"/>
-      <c r="E60" s="37"/>
-      <c r="F60" s="38"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="4">
-        <v>45</v>
-      </c>
-      <c r="B61" s="35"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="37"/>
-      <c r="F61" s="38"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="4">
-        <v>46</v>
-      </c>
-      <c r="B62" s="35"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="39"/>
-      <c r="E62" s="37"/>
-      <c r="F62" s="38"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="4">
-        <v>47</v>
-      </c>
-      <c r="B63" s="35"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="39"/>
-      <c r="E63" s="37"/>
-      <c r="F63" s="38"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="4">
-        <v>48</v>
-      </c>
-      <c r="B64" s="35"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="39"/>
-      <c r="E64" s="37"/>
-      <c r="F64" s="38"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="4">
-        <v>49</v>
-      </c>
-      <c r="B65" s="35"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="39"/>
-      <c r="E65" s="37"/>
-      <c r="F65" s="38"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="4">
-        <v>50</v>
-      </c>
-      <c r="B66" s="35"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="39"/>
-      <c r="E66" s="37"/>
-      <c r="F66" s="38"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="4">
-        <v>51</v>
-      </c>
-      <c r="B67" s="35"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="39"/>
-      <c r="E67" s="37"/>
-      <c r="F67" s="38"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="4">
-        <v>52</v>
-      </c>
-      <c r="B68" s="35"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="39"/>
-      <c r="E68" s="37"/>
-      <c r="F68" s="38"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="4">
-        <v>53</v>
-      </c>
-      <c r="B69" s="35"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="39"/>
-      <c r="E69" s="37"/>
-      <c r="F69" s="38"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="4">
-        <v>54</v>
-      </c>
-      <c r="B70" s="35"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="39"/>
-      <c r="E70" s="37"/>
-      <c r="F70" s="38"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="4">
-        <v>55</v>
-      </c>
-      <c r="B71" s="35"/>
-      <c r="C71" s="4"/>
-      <c r="D71" s="39"/>
-      <c r="E71" s="37"/>
-      <c r="F71" s="38"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="4">
-        <v>56</v>
-      </c>
-      <c r="B72" s="35"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="39"/>
-      <c r="E72" s="37"/>
-      <c r="F72" s="38"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="4">
-        <v>57</v>
-      </c>
-      <c r="B73" s="35"/>
-      <c r="C73" s="4"/>
-      <c r="D73" s="39"/>
-      <c r="E73" s="37"/>
-      <c r="F73" s="38"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="4">
-        <v>58</v>
-      </c>
-      <c r="B74" s="35"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="39"/>
-      <c r="E74" s="37"/>
-      <c r="F74" s="38"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="4">
-        <v>59</v>
-      </c>
-      <c r="B75" s="35"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="39"/>
-      <c r="E75" s="37"/>
-      <c r="F75" s="38"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="4">
-        <v>60</v>
-      </c>
-      <c r="B76" s="35"/>
-      <c r="C76" s="4"/>
-      <c r="D76" s="39"/>
-      <c r="E76" s="37"/>
-      <c r="F76" s="38"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="4">
-        <v>61</v>
-      </c>
-      <c r="B77" s="35"/>
-      <c r="C77" s="4"/>
-      <c r="D77" s="39"/>
-      <c r="E77" s="37"/>
-      <c r="F77" s="38"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="4">
-        <v>62</v>
-      </c>
-      <c r="B78" s="35"/>
-      <c r="C78" s="4"/>
-      <c r="D78" s="39"/>
-      <c r="E78" s="37"/>
-      <c r="F78" s="38"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="4">
-        <v>63</v>
-      </c>
-      <c r="B79" s="35"/>
-      <c r="C79" s="4"/>
-      <c r="D79" s="39"/>
-      <c r="E79" s="37"/>
-      <c r="F79" s="38"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="4">
-        <v>64</v>
-      </c>
-      <c r="B80" s="35"/>
-      <c r="C80" s="4"/>
-      <c r="D80" s="39"/>
-      <c r="E80" s="37"/>
-      <c r="F80" s="38"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="4">
-        <v>65</v>
-      </c>
-      <c r="B81" s="35"/>
-      <c r="C81" s="4"/>
-      <c r="D81" s="39"/>
-      <c r="E81" s="37"/>
-      <c r="F81" s="38"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="4">
-        <v>66</v>
-      </c>
-      <c r="B82" s="35"/>
-      <c r="C82" s="4"/>
-      <c r="D82" s="39"/>
-      <c r="E82" s="37"/>
-      <c r="F82" s="38"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="4">
-        <v>67</v>
-      </c>
-      <c r="B83" s="35"/>
-      <c r="C83" s="4"/>
-      <c r="D83" s="39"/>
-      <c r="E83" s="37"/>
-      <c r="F83" s="38"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" s="4">
-        <v>68</v>
-      </c>
-      <c r="B84" s="35"/>
-      <c r="C84" s="4"/>
-      <c r="D84" s="39"/>
-      <c r="E84" s="37"/>
-      <c r="F84" s="38"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="4">
-        <v>69</v>
-      </c>
-      <c r="B85" s="35"/>
-      <c r="C85" s="4"/>
-      <c r="D85" s="39"/>
-      <c r="E85" s="37"/>
-      <c r="F85" s="38"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="4">
-        <v>70</v>
-      </c>
-      <c r="B86" s="35"/>
-      <c r="C86" s="4"/>
-      <c r="D86" s="39"/>
-      <c r="E86" s="37"/>
-      <c r="F86" s="38"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="4">
-        <v>71</v>
-      </c>
-      <c r="B87" s="35"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="39"/>
-      <c r="E87" s="37"/>
-      <c r="F87" s="38"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="4">
-        <v>72</v>
-      </c>
-      <c r="B88" s="35"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="39"/>
-      <c r="E88" s="37"/>
-      <c r="F88" s="38"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="4">
-        <v>73</v>
-      </c>
-      <c r="B89" s="35"/>
-      <c r="C89" s="4"/>
-      <c r="D89" s="39"/>
-      <c r="E89" s="37"/>
-      <c r="F89" s="38"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="4">
-        <v>74</v>
-      </c>
-      <c r="B90" s="35"/>
-      <c r="C90" s="4"/>
-      <c r="D90" s="39"/>
-      <c r="E90" s="37"/>
-      <c r="F90" s="38"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91" s="4">
-        <v>75</v>
-      </c>
-      <c r="B91" s="35"/>
-      <c r="C91" s="4"/>
-      <c r="D91" s="39"/>
-      <c r="E91" s="37"/>
-      <c r="F91" s="38"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92" s="4">
-        <v>76</v>
-      </c>
-      <c r="B92" s="35"/>
-      <c r="C92" s="4"/>
-      <c r="D92" s="39"/>
-      <c r="E92" s="37"/>
-      <c r="F92" s="38"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93" s="4">
-        <v>77</v>
-      </c>
-      <c r="B93" s="35"/>
-      <c r="C93" s="4"/>
-      <c r="D93" s="39"/>
-      <c r="E93" s="37"/>
-      <c r="F93" s="38"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94" s="4">
-        <v>78</v>
-      </c>
-      <c r="B94" s="35"/>
-      <c r="C94" s="4"/>
-      <c r="D94" s="39"/>
-      <c r="E94" s="37"/>
-      <c r="F94" s="38"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="4">
-        <v>79</v>
-      </c>
-      <c r="B95" s="35"/>
-      <c r="C95" s="4"/>
-      <c r="D95" s="39"/>
-      <c r="E95" s="37"/>
-      <c r="F95" s="38"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="4">
-        <v>80</v>
-      </c>
-      <c r="B96" s="35"/>
-      <c r="C96" s="4"/>
-      <c r="D96" s="39"/>
-      <c r="E96" s="37"/>
-      <c r="F96" s="38"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="4">
-        <v>81</v>
-      </c>
-      <c r="B97" s="35"/>
-      <c r="C97" s="4"/>
-      <c r="D97" s="39"/>
-      <c r="E97" s="37"/>
-      <c r="F97" s="38"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98" s="4">
-        <v>82</v>
-      </c>
-      <c r="B98" s="35"/>
-      <c r="C98" s="4"/>
-      <c r="D98" s="39"/>
-      <c r="E98" s="37"/>
-      <c r="F98" s="38"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99" s="4">
-        <v>83</v>
-      </c>
-      <c r="B99" s="35"/>
-      <c r="C99" s="4"/>
-      <c r="D99" s="39"/>
-      <c r="E99" s="37"/>
-      <c r="F99" s="38"/>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" s="4">
-        <v>84</v>
-      </c>
-      <c r="B100" s="35"/>
-      <c r="C100" s="4"/>
-      <c r="D100" s="39"/>
-      <c r="E100" s="37"/>
-      <c r="F100" s="38"/>
-    </row>
-  </sheetData>
-  <dataValidations count="4">
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task ID" prompt="This is just an arbitrary unique (per sprint) integer assigned to a task, used by the team to refer to that task. " sqref="A17:A100" xr:uid="{00000000-0002-0000-0300-000000000000}">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task Description" prompt="Select a Feature ID to the left. Then, in this column, list each discrete task needed to implement that feature._x000a__x000a_Example tasks might be &quot;create the Foo class&quot;, &quot;add the Bar method to the (existing) Qux class&quot;, &quot;Find icons for the task bar&quot;, &quot;Update the m" sqref="D18:D100" xr:uid="{00000000-0002-0000-0300-000003000000}">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" promptTitle="Implementation Status" prompt="Leave blank until task is begun._x000a_Select &quot;In Work&quot; when started (for long tasks only)._x000a_Select Completed ONLY when this task is done._x000a_    Select &quot;Completed Day 1&quot; if finished on the first day, and_x000a_    similarly for &quot;Completed on Day 2&quot; et. al." sqref="E17:E100" xr:uid="{00000000-0002-0000-0300-000004000000}">
-      <formula1>"In Work,Completed Day 1,Completed Day 2,Completed Day 3,Completed Day 4,Completed Day 5,Completed Day 6,Completed Day 7"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="OPTIONAL" prompt="You may add any notes here that help understand the requirements and scope for this task" sqref="F17:F100" xr:uid="{00000000-0002-0000-0300-000005000000}">
-      <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="Exactly ONE team member may be responsible for any task, and they will receive grade credit for their work._x000a__x000a_If you have more than one person on your team, each member MUST select their initials for each task the agree to perform. Use this to ensure that " xr:uid="{00000000-0002-0000-0300-000002000000}">
-          <x14:formula1>
-            <xm:f>'Product Backlog'!$H$5:$H$9</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>C17:C100</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="The list contains the Feature IDs from the same column on the Product Backlog tab._x000a__x000a_For each (ahem) Feature ID, create one or more rows in this table representing the tasks you need to complete to implement that feature._x000a__x000a_For example, for a &quot;Provide Help " xr:uid="{00000000-0002-0000-0300-000001000000}">
-          <x14:formula1>
-            <xm:f>'Product Backlog'!$A$24:$A$100</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>B17:B100</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Added onSaveClick and onSaveAsClick
</commit_message>
<xml_diff>
--- a/P07/Scrum_Sprint_2.xlsx
+++ b/P07/Scrum_Sprint_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcnar\Desktop\cse1325\P07\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Support\Desktop\cse1325\P07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758A2890-A5FE-4F94-BC41-BA75DBDB9D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6A4494-0D57-49CF-BCDE-C2B3DE0E3702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27105" yWindow="1110" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="217">
   <si>
     <t>Product Name:</t>
   </si>
@@ -662,34 +662,37 @@
     <t>Create turtle image using template in 1325-prof</t>
   </si>
   <si>
+    <t>Create Empty action listeners</t>
+  </si>
+  <si>
+    <t>Populate action listeners</t>
+  </si>
+  <si>
+    <t>Find Photos for toolbar and add them</t>
+  </si>
+  <si>
+    <t>Create and Populate Save method in Customer.java</t>
+  </si>
+  <si>
+    <t>Create and Populate Save method in Option.java</t>
+  </si>
+  <si>
+    <t>Create and Populate Save method in Computer.java</t>
+  </si>
+  <si>
+    <t>Create and populate Save method in Store.java</t>
+  </si>
+  <si>
+    <t>Populate onSaveClick()</t>
+  </si>
+  <si>
+    <t>Populate onSaveAsClick()</t>
+  </si>
+  <si>
+    <t>Populate onNewClick()</t>
+  </si>
+  <si>
     <t>In Work</t>
-  </si>
-  <si>
-    <t>Create Empty action listeners</t>
-  </si>
-  <si>
-    <t>Populate action listeners</t>
-  </si>
-  <si>
-    <t>Find Photos for toolbar and add them</t>
-  </si>
-  <si>
-    <t>Create and Populate Save method in Customer.java</t>
-  </si>
-  <si>
-    <t>Create and Populate Save method in Option.java</t>
-  </si>
-  <si>
-    <t>Create and Populate Save method in Computer.java</t>
-  </si>
-  <si>
-    <t>Create and populate Save method in Store.java</t>
-  </si>
-  <si>
-    <t>Populate onSaveClick()</t>
-  </si>
-  <si>
-    <t>Populate onSaveAsClick()</t>
   </si>
 </sst>
 </file>
@@ -1231,13 +1234,13 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1522,28 +1525,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3885,7 +3888,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3898,8 +3901,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="H50" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4157,11 +4160,11 @@
       </c>
       <c r="B15" s="5">
         <f>B14-C15</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C15" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 3")</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="5"/>
@@ -4181,7 +4184,7 @@
       </c>
       <c r="B16" s="5">
         <f>B15-C16</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C16" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 4")</f>
@@ -4201,7 +4204,7 @@
       </c>
       <c r="B17" s="5">
         <f>B16-C17</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C17" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 4")</f>
@@ -4755,7 +4758,7 @@
         <v>3</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H37" s="18" t="s">
         <v>79</v>
@@ -4787,7 +4790,9 @@
       <c r="F38" s="17">
         <v>3</v>
       </c>
-      <c r="G38" s="17"/>
+      <c r="G38" s="17" t="s">
+        <v>204</v>
+      </c>
       <c r="H38" s="18" t="s">
         <v>79</v>
       </c>
@@ -4818,7 +4823,9 @@
       <c r="F39" s="17">
         <v>3</v>
       </c>
-      <c r="G39" s="17"/>
+      <c r="G39" s="17" t="s">
+        <v>204</v>
+      </c>
       <c r="H39" s="18" t="s">
         <v>79</v>
       </c>
@@ -4849,7 +4856,9 @@
       <c r="F40" s="17">
         <v>3</v>
       </c>
-      <c r="G40" s="17"/>
+      <c r="G40" s="17" t="s">
+        <v>216</v>
+      </c>
       <c r="H40" s="18" t="s">
         <v>79</v>
       </c>
@@ -5870,8 +5879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView topLeftCell="A18" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5976,7 +5985,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -5991,7 +6000,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -6009,11 +6018,11 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
@@ -6027,7 +6036,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -6045,7 +6054,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -6063,7 +6072,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -6081,7 +6090,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -6099,7 +6108,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -6208,7 +6217,7 @@
         <v>156</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E21" s="37" t="s">
         <v>158</v>
@@ -6226,7 +6235,7 @@
         <v>156</v>
       </c>
       <c r="D22" s="39" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E22" s="37" t="s">
         <v>158</v>
@@ -6244,7 +6253,7 @@
         <v>156</v>
       </c>
       <c r="D23" s="39" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E23" s="37" t="s">
         <v>158</v>
@@ -6262,7 +6271,7 @@
         <v>156</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E24" s="37" t="s">
         <v>158</v>
@@ -6280,7 +6289,7 @@
         <v>156</v>
       </c>
       <c r="D25" s="39" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E25" s="37" t="s">
         <v>158</v>
@@ -6298,7 +6307,7 @@
         <v>156</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E26" s="37" t="s">
         <v>158</v>
@@ -6316,7 +6325,7 @@
         <v>156</v>
       </c>
       <c r="D27" s="39" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E27" s="37" t="s">
         <v>158</v>
@@ -6334,7 +6343,7 @@
         <v>156</v>
       </c>
       <c r="D28" s="39" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E28" s="37" t="s">
         <v>158</v>
@@ -6345,15 +6354,9 @@
       <c r="A29" s="4">
         <v>13</v>
       </c>
-      <c r="B29" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D29" s="39" t="s">
-        <v>215</v>
-      </c>
+      <c r="B29" s="35"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="39"/>
       <c r="E29" s="37"/>
       <c r="F29" s="38"/>
     </row>
@@ -6361,10 +6364,18 @@
       <c r="A30" s="4">
         <v>14</v>
       </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="37"/>
+      <c r="B30" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D30" s="39" t="s">
+        <v>214</v>
+      </c>
+      <c r="E30" s="37" t="s">
+        <v>173</v>
+      </c>
       <c r="F30" s="38"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -6381,10 +6392,18 @@
       <c r="A32" s="4">
         <v>16</v>
       </c>
-      <c r="B32" s="35"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="37"/>
+      <c r="B32" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D32" s="39" t="s">
+        <v>215</v>
+      </c>
+      <c r="E32" s="37" t="s">
+        <v>173</v>
+      </c>
       <c r="F32" s="38"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Final Commit for P07
</commit_message>
<xml_diff>
--- a/P07/Scrum_Sprint_2.xlsx
+++ b/P07/Scrum_Sprint_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Support\Desktop\cse1325\P07\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6A4494-0D57-49CF-BCDE-C2B3DE0E3702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16E9849-2756-4701-B63C-2435DCC98905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="30" windowWidth="28770" windowHeight="15570" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="219">
   <si>
     <t>Product Name:</t>
   </si>
@@ -692,7 +692,13 @@
     <t>Populate onNewClick()</t>
   </si>
   <si>
-    <t>In Work</t>
+    <t>Create load constructers for all classes required in spring 3</t>
+  </si>
+  <si>
+    <t>Populate constructers</t>
+  </si>
+  <si>
+    <t>Test program with save, saveas, and load</t>
   </si>
 </sst>
 </file>
@@ -1234,13 +1240,13 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1525,10 +1531,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3901,8 +3907,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4160,11 +4166,11 @@
       </c>
       <c r="B15" s="5">
         <f>B14-C15</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 3")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="5"/>
@@ -4184,7 +4190,7 @@
       </c>
       <c r="B16" s="5">
         <f>B15-C16</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 4")</f>
@@ -4204,7 +4210,7 @@
       </c>
       <c r="B17" s="5">
         <f>B16-C17</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" s="9">
         <f>COUNTIF(G$24:G$106,"Finished in Sprint 4")</f>
@@ -4857,7 +4863,7 @@
         <v>3</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="H40" s="18" t="s">
         <v>79</v>
@@ -5879,8 +5885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView topLeftCell="A15" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5985,7 +5991,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -6000,7 +6006,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -6022,7 +6028,7 @@
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
@@ -6420,30 +6426,54 @@
       <c r="A34" s="4">
         <v>18</v>
       </c>
-      <c r="B34" s="35"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="37"/>
+      <c r="B34" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D34" s="39" t="s">
+        <v>216</v>
+      </c>
+      <c r="E34" s="37" t="s">
+        <v>173</v>
+      </c>
       <c r="F34" s="38"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>19</v>
       </c>
-      <c r="B35" s="35"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="37"/>
+      <c r="B35" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D35" s="39" t="s">
+        <v>217</v>
+      </c>
+      <c r="E35" s="37" t="s">
+        <v>173</v>
+      </c>
       <c r="F35" s="38"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>20</v>
       </c>
-      <c r="B36" s="35"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="39"/>
-      <c r="E36" s="37"/>
+      <c r="B36" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D36" s="39" t="s">
+        <v>218</v>
+      </c>
+      <c r="E36" s="37" t="s">
+        <v>173</v>
+      </c>
       <c r="F36" s="38"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>